<commit_message>
Added specs for current behavior with empty trailing rows
</commit_message>
<xml_diff>
--- a/test/files/simple_spreadsheet_empty_cells.xlsx
+++ b/test/files/simple_spreadsheet_empty_cells.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/julien/Dev/Projects/textmaster/libraries/roo/test/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13188D8D-DB74-A847-B816-8739376098E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{845C6885-B55B-8749-8E82-C6CDA0103635}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22720" yWindow="5280" windowWidth="27640" windowHeight="16940" xr2:uid="{A4162F49-0BE1-F942-AAFC-D0EE2F974F07}"/>
+    <workbookView xWindow="12140" yWindow="5280" windowWidth="27640" windowHeight="16940" xr2:uid="{A4162F49-0BE1-F942-AAFC-D0EE2F974F07}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -102,7 +102,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -110,17 +110,28 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -139,7 +150,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -427,7 +438,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -435,10 +446,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04B0325E-0BDA-4344-9B4D-A157AF5B466B}">
-  <dimension ref="A3:F12"/>
+  <dimension ref="A3:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -544,6 +555,12 @@
         <v>9</v>
       </c>
     </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="6"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
+    </row>
+    <row r="16" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Never stream trailing empty rows
</commit_message>
<xml_diff>
--- a/test/files/simple_spreadsheet_empty_cells.xlsx
+++ b/test/files/simple_spreadsheet_empty_cells.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/julien/Dev/Projects/textmaster/libraries/roo/test/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{845C6885-B55B-8749-8E82-C6CDA0103635}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B3EB4CD-266D-9342-943F-D827058E6F0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12140" yWindow="5280" windowWidth="27640" windowHeight="16940" xr2:uid="{A4162F49-0BE1-F942-AAFC-D0EE2F974F07}"/>
   </bookViews>
@@ -123,7 +123,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -131,7 +131,8 @@
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -446,10 +447,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04B0325E-0BDA-4344-9B4D-A157AF5B466B}">
-  <dimension ref="A3:F16"/>
+  <dimension ref="A3:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -514,13 +515,13 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="3">
+      <c r="A10" s="7">
         <v>39210</v>
       </c>
-      <c r="B10" s="4">
+      <c r="B10" s="8">
         <v>10.75</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C10" s="8">
         <v>12.75</v>
       </c>
       <c r="E10" t="s">
@@ -555,12 +556,11 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="6"/>
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
-    </row>
-    <row r="16" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="6"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>